<commit_message>
eddy ni 1996-1997 (update)
</commit_message>
<xml_diff>
--- a/_data/ni/ni9697/individueel_eindstand_dworp_123_9697.xlsx
+++ b/_data/ni/ni9697/individueel_eindstand_dworp_123_9697.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14520" windowHeight="12840" activeTab="7"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14520" windowHeight="12840" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="242">
   <si>
     <t>Jaar 1</t>
   </si>
@@ -526,9 +526,6 @@
     <t>Pitropakis Anthony</t>
   </si>
   <si>
-    <t>473 Aalter</t>
-  </si>
-  <si>
     <t>De Lathouwer Marc</t>
   </si>
   <si>
@@ -728,6 +725,33 @@
   </si>
   <si>
     <t>Carpentier Claude</t>
+  </si>
+  <si>
+    <t>473 Pion Aalter</t>
+  </si>
+  <si>
+    <t>R1 Dworp 3:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pion Aalter? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>intussen opgedoekt; ev. gefusioneerd mer Doorbraak Aalter (zie ronde 9)?</t>
+  </si>
+  <si>
+    <t>R6 Dworp 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">naschrift   R6 naschrift Thibucle ipv Tibucle  </t>
+  </si>
+  <si>
+    <t>Er is een verschik tussen kring 244 Thibucle en kring 272 Tibéchecs; zie JV 1997-1998 ploegresultaten Dworp 1</t>
   </si>
 </sst>
 </file>
@@ -1824,10 +1848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:E13"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1891,7 +1915,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="B10" s="68" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C10" s="69"/>
       <c r="D10" s="69"/>
@@ -1915,11 +1939,77 @@
     </row>
     <row r="14" spans="1:9">
       <c r="B14" s="70" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C14" s="70"/>
       <c r="D14" s="70"/>
       <c r="E14" s="70"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" t="s">
+        <v>235</v>
+      </c>
+      <c r="C17" t="s">
+        <v>236</v>
+      </c>
+      <c r="D17" t="s">
+        <v>236</v>
+      </c>
+      <c r="E17" t="s">
+        <v>236</v>
+      </c>
+      <c r="F17" t="s">
+        <v>236</v>
+      </c>
+      <c r="G17" t="s">
+        <v>236</v>
+      </c>
+      <c r="H17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C21" t="s">
+        <v>236</v>
+      </c>
+      <c r="D21" t="s">
+        <v>236</v>
+      </c>
+      <c r="E21" t="s">
+        <v>236</v>
+      </c>
+      <c r="F21" t="s">
+        <v>236</v>
+      </c>
+      <c r="G21" t="s">
+        <v>236</v>
+      </c>
+      <c r="H21" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" t="s">
+        <v>241</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1930,7 +2020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -2118,7 +2208,7 @@
         <v>31496</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>48</v>
@@ -2315,7 +2405,7 @@
         <v>1858</v>
       </c>
       <c r="L16" s="70" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M16" s="70"/>
       <c r="N16" s="70"/>
@@ -2360,7 +2450,7 @@
         <v>1844</v>
       </c>
       <c r="L17" s="69" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M17" s="69"/>
       <c r="N17" s="69"/>
@@ -2439,7 +2529,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2491,7 +2581,7 @@
         <v>27227</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D23" s="18">
         <v>1888</v>
@@ -2523,7 +2613,7 @@
         <v>34835</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D24" s="18">
         <v>1791</v>
@@ -2555,7 +2645,7 @@
         <v>35181</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>48</v>
@@ -2587,7 +2677,7 @@
         <v>56243</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>48</v>
@@ -3265,7 +3355,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -3325,7 +3415,7 @@
         <v>16748</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J23" s="18">
         <v>1741</v>
@@ -3357,7 +3447,7 @@
         <v>7277</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J24" s="18">
         <v>1626</v>
@@ -3389,7 +3479,7 @@
         <v>41556</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J25" s="18">
         <v>1507</v>
@@ -3421,7 +3511,7 @@
         <v>5347</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J26" s="18">
         <v>1447</v>
@@ -3988,7 +4078,7 @@
         <v>91014</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D17" s="18">
         <v>1667</v>
@@ -4079,7 +4169,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -4131,7 +4221,7 @@
         <v>41114</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D23" s="18">
         <v>1628</v>
@@ -4163,7 +4253,7 @@
         <v>48909</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D24" s="18">
         <v>1543</v>
@@ -4195,7 +4285,7 @@
         <v>48879</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D25" s="18">
         <v>1482</v>
@@ -4227,7 +4317,7 @@
         <v>50458</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>48</v>
@@ -4531,7 +4621,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C4" s="40" t="s">
         <v>37</v>
@@ -4660,7 +4750,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C5" s="41"/>
       <c r="D5" s="40" t="s">
@@ -4789,7 +4879,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
@@ -4918,7 +5008,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C7" s="41"/>
       <c r="D7" s="41"/>
@@ -5047,7 +5137,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C8" s="41"/>
       <c r="D8" s="41"/>
@@ -5176,7 +5266,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C9" s="41"/>
       <c r="D9" s="41"/>
@@ -5305,7 +5395,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C10" s="41"/>
       <c r="D10" s="41"/>
@@ -5434,7 +5524,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C11" s="41"/>
       <c r="D11" s="41"/>
@@ -5563,7 +5653,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C12" s="41"/>
       <c r="D12" s="41"/>
@@ -5692,7 +5782,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
@@ -5821,7 +5911,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C14" s="41"/>
       <c r="D14" s="41"/>
@@ -5950,7 +6040,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C15" s="46"/>
       <c r="D15" s="46"/>
@@ -6173,7 +6263,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>37</v>
@@ -6302,7 +6392,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C19" s="41"/>
       <c r="D19" s="40" t="s">
@@ -6431,7 +6521,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C20" s="41"/>
       <c r="D20" s="41"/>
@@ -6560,7 +6650,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C21" s="41"/>
       <c r="D21" s="41"/>
@@ -6689,7 +6779,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C22" s="41"/>
       <c r="D22" s="41"/>
@@ -6818,7 +6908,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C23" s="41"/>
       <c r="D23" s="41"/>
@@ -6947,7 +7037,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C24" s="41"/>
       <c r="D24" s="41"/>
@@ -7076,7 +7166,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C25" s="41"/>
       <c r="D25" s="41"/>
@@ -7205,7 +7295,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C26" s="41"/>
       <c r="D26" s="41"/>
@@ -7334,7 +7424,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C27" s="41"/>
       <c r="D27" s="41"/>
@@ -7463,7 +7553,7 @@
         <v>11</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C28" s="41"/>
       <c r="D28" s="41"/>
@@ -7592,7 +7682,7 @@
         <v>12</v>
       </c>
       <c r="B29" s="45" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C29" s="46"/>
       <c r="D29" s="46"/>
@@ -7815,7 +7905,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C32" s="40" t="s">
         <v>37</v>
@@ -7944,7 +8034,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C33" s="41"/>
       <c r="D33" s="40" t="s">
@@ -8073,7 +8163,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C34" s="41"/>
       <c r="D34" s="41"/>
@@ -8202,7 +8292,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C35" s="41"/>
       <c r="D35" s="41"/>
@@ -8331,7 +8421,7 @@
         <v>5</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C36" s="41"/>
       <c r="D36" s="41"/>
@@ -8460,7 +8550,7 @@
         <v>6</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C37" s="41"/>
       <c r="D37" s="41"/>
@@ -8589,7 +8679,7 @@
         <v>7</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C38" s="41"/>
       <c r="D38" s="41"/>
@@ -8718,7 +8808,7 @@
         <v>8</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C39" s="41"/>
       <c r="D39" s="41"/>
@@ -8847,7 +8937,7 @@
         <v>9</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C40" s="41"/>
       <c r="D40" s="41"/>
@@ -8976,7 +9066,7 @@
         <v>10</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C41" s="41"/>
       <c r="D41" s="41"/>
@@ -9105,7 +9195,7 @@
         <v>11</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C42" s="41"/>
       <c r="D42" s="41"/>
@@ -9234,7 +9324,7 @@
         <v>12</v>
       </c>
       <c r="B43" s="45" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C43" s="46"/>
       <c r="D43" s="46"/>
@@ -14108,7 +14198,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14582,7 +14672,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>166</v>
+        <v>233</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -14632,7 +14722,7 @@
         <v>47341</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D23" s="18">
         <v>1776</v>
@@ -14664,7 +14754,7 @@
         <v>44938</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D24" s="18">
         <v>1768</v>
@@ -14696,7 +14786,7 @@
         <v>66737</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D25" s="18">
         <v>1627</v>
@@ -14714,7 +14804,7 @@
         <v>4014</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J25" s="18">
         <v>1639</v>
@@ -14728,7 +14818,7 @@
         <v>11096</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>48</v>
@@ -14970,7 +15060,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -15404,7 +15494,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -15464,7 +15554,7 @@
         <v>96491</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J23" s="18">
         <v>1719</v>
@@ -15496,7 +15586,7 @@
         <v>58114</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J24" s="18">
         <v>1487</v>
@@ -15528,7 +15618,7 @@
         <v>96440</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J25" s="18">
         <v>1566</v>
@@ -15542,7 +15632,7 @@
         <v>12769</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>48</v>
@@ -15560,7 +15650,7 @@
         <v>72036</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J26" s="18">
         <v>1425</v>
@@ -16210,7 +16300,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -16260,7 +16350,7 @@
         <v>2658</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D23" s="18">
         <v>1475</v>
@@ -16292,7 +16382,7 @@
         <v>11568</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D24" s="18">
         <v>1409</v>
@@ -16324,7 +16414,7 @@
         <v>6564</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D25" s="18">
         <v>1362</v>
@@ -16356,7 +16446,7 @@
         <v>15652</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>48</v>
@@ -17032,7 +17122,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -17092,7 +17182,7 @@
         <v>55441</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J23" s="18">
         <v>1717</v>
@@ -17124,7 +17214,7 @@
         <v>38741</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J24" s="18">
         <v>1604</v>
@@ -17156,7 +17246,7 @@
         <v>33588</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J25" s="18">
         <v>1451</v>
@@ -17188,7 +17278,7 @@
         <v>19828</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J26" s="18">
         <v>1444</v>
@@ -17633,7 +17723,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -17838,7 +17928,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -17888,7 +17978,7 @@
         <v>33421</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D23" s="18">
         <v>1781</v>
@@ -17920,7 +18010,7 @@
         <v>44466</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D24" s="18">
         <v>1777</v>
@@ -17952,7 +18042,7 @@
         <v>49794</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D25" s="18">
         <v>1669</v>
@@ -17984,7 +18074,7 @@
         <v>33472</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D26" s="18">
         <v>1434</v>
@@ -18450,7 +18540,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -18655,7 +18745,7 @@
         <v>11</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -18715,7 +18805,7 @@
         <v>21300</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J23" s="18">
         <v>1735</v>
@@ -18747,7 +18837,7 @@
         <v>51535</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J24" s="18" t="s">
         <v>48</v>
@@ -18779,7 +18869,7 @@
         <v>10588</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J25" s="18" t="s">
         <v>48</v>
@@ -18811,7 +18901,7 @@
         <v>51454</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J26" s="18" t="s">
         <v>48</v>
@@ -18986,7 +19076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -19467,7 +19557,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -19517,7 +19607,7 @@
         <v>32468</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D23" s="18">
         <v>1305</v>
@@ -19549,7 +19639,7 @@
         <v>24261</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D24" s="18">
         <v>1176</v>
@@ -19581,7 +19671,7 @@
         <v>31500</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D25" s="18">
         <v>1079</v>
@@ -19613,7 +19703,7 @@
         <v>37583</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>48</v>
@@ -20084,7 +20174,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -20289,7 +20379,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -20349,7 +20439,7 @@
         <v>58211</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J23" s="18">
         <v>1600</v>
@@ -20381,7 +20471,7 @@
         <v>37435</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J24" s="18">
         <v>1535</v>
@@ -20413,7 +20503,7 @@
         <v>22284</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J25" s="18">
         <v>1453</v>
@@ -20445,7 +20535,7 @@
         <v>6882</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J26" s="18">
         <v>1363</v>

</xml_diff>

<commit_message>
OSK is Ons Schaakgenoegen Kempen
</commit_message>
<xml_diff>
--- a/_data/ni/ni9697/individueel_eindstand_dworp_123_9697.xlsx
+++ b/_data/ni/ni9697/individueel_eindstand_dworp_123_9697.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14340" yWindow="-15" windowWidth="14385" windowHeight="12870" activeTab="12"/>
+    <workbookView xWindow="-30" yWindow="-30" windowWidth="14385" windowHeight="12870"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="259">
   <si>
     <t>Jaar 1</t>
   </si>
@@ -601,9 +601,6 @@
     <t>Verbraeken Lucien</t>
   </si>
   <si>
-    <t>186 OSK 6</t>
-  </si>
-  <si>
     <t>Huysmans Jos</t>
   </si>
   <si>
@@ -776,6 +773,36 @@
   </si>
   <si>
     <t>matchpunten: w 3 - g 2 - v 1 - vf 0</t>
+  </si>
+  <si>
+    <t>186 Ons Schaakgenoegen Kempen 6</t>
+  </si>
+  <si>
+    <t>186 OSK is Ons Schaakgenoegen Kempen, 186 was het stamnummer van Tessenderlo (bron Sylvin De Vet)</t>
+  </si>
+  <si>
+    <t>Het idee was o.a. om een sterke ploeg in 1ste nationale te krijgen, wat ook lukte.</t>
+  </si>
+  <si>
+    <t>Er zat een Vzw achter (pieter: waarschijnlijk  Ons Schaakgenoegen, opgericht in maart 1994), opgericht door 4 personen</t>
+  </si>
+  <si>
+    <t>Dat laatste werd uiteindelijk het probleem en de ondergang van de club.</t>
+  </si>
+  <si>
+    <t>De club ging rond 2000 nog samen met KASK tot KAOSK, maar dat werkte niet met 2 gescheiden groepen:</t>
+  </si>
+  <si>
+    <t>1 in Antwerpen en 1 in de Kempen.</t>
+  </si>
+  <si>
+    <t>Drijvende kracht was Cies Gysen, die volgens Sylvin veel goede ideeën had, maar ook mensen die dit voor hem wilden uitvoeren.</t>
+  </si>
+  <si>
+    <t>Ze speelden niet alleen NI, maar ook Zilveren Toren (tornooi Liga Antwerpen)</t>
+  </si>
+  <si>
+    <t>Het was het samenwerken van Tessenderlo, Mol en Geel. Tessenderlo en Mol waren toen clubs in moeilijkheden.</t>
   </si>
 </sst>
 </file>
@@ -1952,10 +1979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1972,7 +1999,7 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="A2" s="64" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2023,13 +2050,13 @@
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="72" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B9" s="73"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="74" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B10" s="75">
         <v>1</v>
@@ -2037,7 +2064,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="74" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B11" s="76">
         <v>0</v>
@@ -2045,7 +2072,7 @@
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" s="74" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B12" s="77">
         <v>0</v>
@@ -2053,7 +2080,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="B13" s="61" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C13" s="62"/>
       <c r="D13" s="62"/>
@@ -2077,7 +2104,7 @@
     </row>
     <row r="17" spans="2:8">
       <c r="B17" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C17" s="63"/>
       <c r="D17" s="63"/>
@@ -2085,70 +2112,115 @@
     </row>
     <row r="18" spans="2:8">
       <c r="B18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="2:8">
       <c r="B20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="2:8">
       <c r="B21" s="78" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D21" t="s">
+        <v>231</v>
+      </c>
+      <c r="E21" t="s">
+        <v>231</v>
+      </c>
+      <c r="F21" t="s">
+        <v>231</v>
+      </c>
+      <c r="G21" t="s">
+        <v>231</v>
+      </c>
+      <c r="H21" t="s">
         <v>232</v>
-      </c>
-      <c r="E21" t="s">
-        <v>232</v>
-      </c>
-      <c r="F21" t="s">
-        <v>232</v>
-      </c>
-      <c r="G21" t="s">
-        <v>232</v>
-      </c>
-      <c r="H21" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="22" spans="2:8">
       <c r="B22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C25" t="s">
+        <v>231</v>
+      </c>
+      <c r="D25" t="s">
+        <v>231</v>
+      </c>
+      <c r="E25" t="s">
+        <v>231</v>
+      </c>
+      <c r="F25" t="s">
+        <v>231</v>
+      </c>
+      <c r="G25" t="s">
+        <v>231</v>
+      </c>
+      <c r="H25" t="s">
         <v>232</v>
-      </c>
-      <c r="D25" t="s">
-        <v>232</v>
-      </c>
-      <c r="E25" t="s">
-        <v>232</v>
-      </c>
-      <c r="F25" t="s">
-        <v>232</v>
-      </c>
-      <c r="G25" t="s">
-        <v>232</v>
-      </c>
-      <c r="H25" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" t="s">
-        <v>237</v>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="B32" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -2346,7 +2418,7 @@
         <v>31496</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>48</v>
@@ -2543,7 +2615,7 @@
         <v>1858</v>
       </c>
       <c r="L16" s="63" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M16" s="63"/>
       <c r="N16" s="63"/>
@@ -2588,7 +2660,7 @@
         <v>1844</v>
       </c>
       <c r="L17" s="62" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M17" s="62"/>
       <c r="N17" s="62"/>
@@ -2667,7 +2739,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2719,7 +2791,7 @@
         <v>27227</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D23" s="18">
         <v>1888</v>
@@ -2751,7 +2823,7 @@
         <v>34835</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D24" s="18">
         <v>1791</v>
@@ -2783,7 +2855,7 @@
         <v>35181</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>48</v>
@@ -2815,7 +2887,7 @@
         <v>56243</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>48</v>
@@ -3499,7 +3571,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -3559,7 +3631,7 @@
         <v>16748</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J23" s="18">
         <v>1741</v>
@@ -3591,7 +3663,7 @@
         <v>7277</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J24" s="18">
         <v>1626</v>
@@ -3623,7 +3695,7 @@
         <v>41556</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J25" s="18">
         <v>1507</v>
@@ -3655,7 +3727,7 @@
         <v>5347</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J26" s="18">
         <v>1447</v>
@@ -4220,7 +4292,7 @@
         <v>91014</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D17" s="18">
         <v>1667</v>
@@ -4311,7 +4383,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -4363,7 +4435,7 @@
         <v>41114</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D23" s="18">
         <v>1628</v>
@@ -4395,7 +4467,7 @@
         <v>48909</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D24" s="18">
         <v>1543</v>
@@ -4427,7 +4499,7 @@
         <v>48879</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D25" s="18">
         <v>1482</v>
@@ -4459,7 +4531,7 @@
         <v>50458</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>48</v>
@@ -4652,7 +4724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BD280"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4681,13 +4753,13 @@
         <v>14</v>
       </c>
       <c r="S2" s="79" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF2" s="80" t="s">
         <v>247</v>
       </c>
-      <c r="AF2" s="80" t="s">
+      <c r="AS2" s="79" t="s">
         <v>248</v>
-      </c>
-      <c r="AS2" s="79" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:56" s="43" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
@@ -7350,7 +7422,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C20" s="34">
         <v>3</v>
@@ -7746,7 +7818,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C22" s="34">
         <v>2.5</v>
@@ -9132,7 +9204,7 @@
         <v>12</v>
       </c>
       <c r="B29" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C29" s="39">
         <v>0</v>
@@ -17301,7 +17373,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -17687,7 +17759,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -19771,7 +19843,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -20378,7 +20450,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -20918,7 +20990,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20931,7 +21003,7 @@
     <col min="6" max="6" width="3.140625" customWidth="1"/>
     <col min="7" max="7" width="5.42578125" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" customWidth="1"/>
+    <col min="9" max="9" width="36" customWidth="1"/>
     <col min="10" max="10" width="6.7109375" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -21203,7 +21275,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -21408,7 +21480,7 @@
         <v>11</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>191</v>
+        <v>249</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -21468,7 +21540,7 @@
         <v>21300</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J23" s="18">
         <v>1735</v>
@@ -21500,7 +21572,7 @@
         <v>51535</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J24" s="18" t="s">
         <v>48</v>
@@ -21532,7 +21604,7 @@
         <v>10588</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J25" s="18" t="s">
         <v>48</v>
@@ -21564,7 +21636,7 @@
         <v>51454</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J26" s="18" t="s">
         <v>48</v>
@@ -22220,7 +22292,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -22270,7 +22342,7 @@
         <v>32468</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D23" s="18">
         <v>1305</v>
@@ -22302,7 +22374,7 @@
         <v>24261</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D24" s="18">
         <v>1176</v>
@@ -22334,7 +22406,7 @@
         <v>31500</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D25" s="18">
         <v>1079</v>
@@ -22366,7 +22438,7 @@
         <v>37583</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>48</v>
@@ -22835,7 +22907,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -23040,7 +23112,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -23100,7 +23172,7 @@
         <v>58211</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J23" s="18">
         <v>1600</v>
@@ -23132,7 +23204,7 @@
         <v>37435</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J24" s="18">
         <v>1535</v>
@@ -23164,7 +23236,7 @@
         <v>22284</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J25" s="18">
         <v>1453</v>
@@ -23196,7 +23268,7 @@
         <v>6882</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J26" s="18">
         <v>1363</v>

</xml_diff>